<commit_message>
even more testing, are certain commands needed?
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/specter/USEquities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC48860-FF02-0348-958B-29354ECDC808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B045E-877F-624A-8E05-23AE2D678E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{0D9173E6-5474-2D4A-B780-40A338A7D577}"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0D9173E6-5474-2D4A-B780-40A338A7D577}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Test Cell</t>
   </si>
@@ -48,6 +49,9 @@
   </si>
   <si>
     <t>additional testing</t>
+  </si>
+  <si>
+    <t>additional test sheet</t>
   </si>
 </sst>
 </file>
@@ -401,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB51E76-B567-DF4A-B389-1FA88E09ADC8}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -431,4 +435,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491E7458-5CCD-9842-9271-4A08EA75A0CD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>